<commit_message>
Update ean codes generation
</commit_message>
<xml_diff>
--- a/excel-files/ean/ean_codes.xlsx
+++ b/excel-files/ean/ean_codes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,28 +443,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4172724086641</t>
+          <t>4517820972430</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>7537180981662</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1202257751562</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>8836976556485</t>
+          <t>4892958240271</t>
         </is>
       </c>
     </row>

</xml_diff>